<commit_message>
latest regressions with data processing
</commit_message>
<xml_diff>
--- a/docs/correlation_matrix.xlsx
+++ b/docs/correlation_matrix.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Rolling_Avg_Misaligned_1M</t>
+          <t>Rolling_Avg_Misaligned_6M</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -510,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02319452792299736</v>
+        <v>0.02435689520289818</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04226782259869653</v>
+        <v>0.04226782259869652</v>
       </c>
       <c r="E2" t="n">
         <v>0.1402561485966509</v>
@@ -525,7 +525,7 @@
         <v>-0.1183523727987073</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.001445324142238785</v>
+        <v>-0.00144532414223878</v>
       </c>
       <c r="I2" t="n">
         <v>0.08176519364168743</v>
@@ -534,7 +534,7 @@
         <v>-0.03738877038550362</v>
       </c>
       <c r="K2" t="n">
-        <v>0.05668574567102286</v>
+        <v>0.05668574567102287</v>
       </c>
       <c r="L2" t="n">
         <v>-0.1169924274199434</v>
@@ -543,53 +543,53 @@
         <v>0.01074723381532353</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.08887914460199314</v>
+        <v>-0.08887914460199312</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rolling_Avg_Misaligned_1M</t>
+          <t>Rolling_Avg_Misaligned_6M</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.02319452792299736</v>
+        <v>0.02435689520289818</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.07290094532089891</v>
+        <v>-0.06928357492136708</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1589670533155016</v>
+        <v>0.1618402499033878</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.02014170342764639</v>
+        <v>-0.01858395782870342</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02596222853965688</v>
+        <v>0.003482931764957531</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001945123397591692</v>
+        <v>0.001884881086372575</v>
       </c>
       <c r="I3" t="n">
-        <v>0.06303790628444358</v>
+        <v>0.06744470724421375</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0449378979343442</v>
+        <v>0.04841034537771964</v>
       </c>
       <c r="K3" t="n">
-        <v>0.05834196619792725</v>
+        <v>0.05565677493390313</v>
       </c>
       <c r="L3" t="n">
-        <v>0.02340578014137535</v>
+        <v>0.01217573226643082</v>
       </c>
       <c r="M3" t="n">
-        <v>0.03902527800672712</v>
+        <v>0.04606925186632603</v>
       </c>
       <c r="N3" t="n">
-        <v>0.04279219720910433</v>
+        <v>0.04579195693789806</v>
       </c>
     </row>
     <row r="4">
@@ -599,34 +599,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.04226782259869653</v>
+        <v>0.04226782259869652</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.07290094532089891</v>
+        <v>-0.06928357492136708</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06149912334035906</v>
+        <v>0.06149912334035905</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02413345473059603</v>
+        <v>0.02413345473059602</v>
       </c>
       <c r="G4" t="n">
         <v>-0.07922568403574144</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.002372091436832226</v>
+        <v>-0.002372091436832229</v>
       </c>
       <c r="I4" t="n">
-        <v>0.05495939966444912</v>
+        <v>0.0549593996644491</v>
       </c>
       <c r="J4" t="n">
         <v>-0.04604720261113404</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0401450241559867</v>
+        <v>0.04014502415598669</v>
       </c>
       <c r="L4" t="n">
         <v>-0.2154371967063657</v>
@@ -635,7 +635,7 @@
         <v>0.1186199138645601</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.01893148487609337</v>
+        <v>-0.01893148487609338</v>
       </c>
     </row>
     <row r="5">
@@ -648,37 +648,37 @@
         <v>0.1402561485966509</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1589670533155016</v>
+        <v>0.1618402499033878</v>
       </c>
       <c r="D5" t="n">
-        <v>0.06149912334035906</v>
+        <v>0.06149912334035905</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.01924531793298756</v>
+        <v>0.01924531793298757</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.01081426358502753</v>
+        <v>-0.01081426358502754</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0007567622585659136</v>
+        <v>-0.0007567622585659154</v>
       </c>
       <c r="I5" t="n">
         <v>0.03959310389554156</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.02065820748257092</v>
+        <v>-0.02065820748257093</v>
       </c>
       <c r="K5" t="n">
-        <v>0.07480425044441925</v>
+        <v>0.07480425044441923</v>
       </c>
       <c r="L5" t="n">
         <v>-0.1491519195044807</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.004832613374206192</v>
+        <v>-0.004832613374206191</v>
       </c>
       <c r="N5" t="n">
         <v>-0.1164410583049517</v>
@@ -694,34 +694,34 @@
         <v>0.01275549834031102</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.02014170342764639</v>
+        <v>-0.01858395782870342</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02413345473059603</v>
+        <v>0.02413345473059602</v>
       </c>
       <c r="E6" t="n">
-        <v>0.01924531793298756</v>
+        <v>0.01924531793298757</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.08181963744959721</v>
+        <v>0.08181963744959719</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.0009238941443531921</v>
+        <v>-0.0009238941443531934</v>
       </c>
       <c r="I6" t="n">
         <v>0.0130842363708376</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.003482285323228753</v>
+        <v>-0.003482285323228752</v>
       </c>
       <c r="K6" t="n">
         <v>0.0593100169700841</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.09351902174369983</v>
+        <v>-0.09351902174369986</v>
       </c>
       <c r="M6" t="n">
         <v>0.01036824121417548</v>
@@ -740,37 +740,37 @@
         <v>-0.1183523727987073</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02596222853965688</v>
+        <v>0.003482931764957531</v>
       </c>
       <c r="D7" t="n">
         <v>-0.07922568403574144</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.01081426358502753</v>
+        <v>-0.01081426358502754</v>
       </c>
       <c r="F7" t="n">
-        <v>0.08181963744959721</v>
+        <v>0.08181963744959719</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.002383877351227505</v>
+        <v>0.002383877351227499</v>
       </c>
       <c r="I7" t="n">
         <v>-0.09862828259620196</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.05987449686194376</v>
+        <v>-0.05987449686194377</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3798642189897708</v>
+        <v>0.3798642189897706</v>
       </c>
       <c r="L7" t="n">
         <v>0.1593863696808671</v>
       </c>
       <c r="M7" t="n">
-        <v>0.03640899503708584</v>
+        <v>0.03640899503708583</v>
       </c>
       <c r="N7" t="n">
         <v>-0.137159322736744</v>
@@ -783,43 +783,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.001445324142238785</v>
+        <v>-0.00144532414223878</v>
       </c>
       <c r="C8" t="n">
-        <v>0.001945123397591692</v>
+        <v>0.001884881086372575</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.002372091436832226</v>
+        <v>-0.002372091436832229</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0007567622585659136</v>
+        <v>-0.0007567622585659154</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.0009238941443531921</v>
+        <v>-0.0009238941443531934</v>
       </c>
       <c r="G8" t="n">
-        <v>0.002383877351227505</v>
+        <v>0.002383877351227499</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>9.61127441443936e-06</v>
+        <v>9.611274414439937e-06</v>
       </c>
       <c r="J8" t="n">
-        <v>0.001063558458272518</v>
+        <v>0.001063558458272517</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.00236731149796097</v>
+        <v>-0.002367311497960982</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0006593989500711889</v>
+        <v>0.0006593989500711931</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.003756267431308732</v>
+        <v>-0.003756267431308731</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0009322909582774888</v>
+        <v>0.0009322909582774932</v>
       </c>
     </row>
     <row r="9">
@@ -832,10 +832,10 @@
         <v>0.08176519364168743</v>
       </c>
       <c r="C9" t="n">
-        <v>0.06303790628444358</v>
+        <v>0.06744470724421375</v>
       </c>
       <c r="D9" t="n">
-        <v>0.05495939966444912</v>
+        <v>0.0549593996644491</v>
       </c>
       <c r="E9" t="n">
         <v>0.03959310389554156</v>
@@ -847,25 +847,25 @@
         <v>-0.09862828259620196</v>
       </c>
       <c r="H9" t="n">
-        <v>9.61127441443936e-06</v>
+        <v>9.611274414439937e-06</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.01978848351359108</v>
+        <v>0.01978848351359107</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1854957068454135</v>
+        <v>0.1854957068454134</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.06405003630667887</v>
+        <v>-0.06405003630667885</v>
       </c>
       <c r="M9" t="n">
-        <v>0.05400895170944195</v>
+        <v>0.05400895170944196</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.02642557985560759</v>
+        <v>-0.0264255798556076</v>
       </c>
     </row>
     <row r="10">
@@ -878,25 +878,25 @@
         <v>-0.03738877038550362</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0449378979343442</v>
+        <v>0.04841034537771964</v>
       </c>
       <c r="D10" t="n">
         <v>-0.04604720261113404</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.02065820748257092</v>
+        <v>-0.02065820748257093</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.003482285323228753</v>
+        <v>-0.003482285323228752</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.05987449686194376</v>
+        <v>-0.05987449686194377</v>
       </c>
       <c r="H10" t="n">
-        <v>0.001063558458272518</v>
+        <v>0.001063558458272517</v>
       </c>
       <c r="I10" t="n">
-        <v>0.01978848351359108</v>
+        <v>0.01978848351359107</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -911,7 +911,7 @@
         <v>0.06973382062536339</v>
       </c>
       <c r="N10" t="n">
-        <v>0.01892521710331612</v>
+        <v>0.01892521710331613</v>
       </c>
     </row>
     <row r="11">
@@ -921,28 +921,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.05668574567102286</v>
+        <v>0.05668574567102287</v>
       </c>
       <c r="C11" t="n">
-        <v>0.05834196619792725</v>
+        <v>0.05565677493390313</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0401450241559867</v>
+        <v>0.04014502415598669</v>
       </c>
       <c r="E11" t="n">
-        <v>0.07480425044441925</v>
+        <v>0.07480425044441923</v>
       </c>
       <c r="F11" t="n">
         <v>0.0593100169700841</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3798642189897708</v>
+        <v>0.3798642189897706</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.00236731149796097</v>
+        <v>-0.002367311497960982</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1854957068454135</v>
+        <v>0.1854957068454134</v>
       </c>
       <c r="J11" t="n">
         <v>-0.02017239516610971</v>
@@ -954,10 +954,10 @@
         <v>-0.06711057455693779</v>
       </c>
       <c r="M11" t="n">
-        <v>0.2987826524325735</v>
+        <v>0.2987826524325734</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.1653177463296435</v>
+        <v>-0.1653177463296434</v>
       </c>
     </row>
     <row r="12">
@@ -970,7 +970,7 @@
         <v>-0.1169924274199434</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02340578014137535</v>
+        <v>0.01217573226643082</v>
       </c>
       <c r="D12" t="n">
         <v>-0.2154371967063657</v>
@@ -979,16 +979,16 @@
         <v>-0.1491519195044807</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.09351902174369983</v>
+        <v>-0.09351902174369986</v>
       </c>
       <c r="G12" t="n">
         <v>0.1593863696808671</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0006593989500711889</v>
+        <v>0.0006593989500711931</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.06405003630667887</v>
+        <v>-0.06405003630667885</v>
       </c>
       <c r="J12" t="n">
         <v>-0.07208363486230991</v>
@@ -1016,31 +1016,31 @@
         <v>0.01074723381532353</v>
       </c>
       <c r="C13" t="n">
-        <v>0.03902527800672712</v>
+        <v>0.04606925186632603</v>
       </c>
       <c r="D13" t="n">
         <v>0.1186199138645601</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.004832613374206192</v>
+        <v>-0.004832613374206191</v>
       </c>
       <c r="F13" t="n">
         <v>0.01036824121417548</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03640899503708584</v>
+        <v>0.03640899503708583</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.003756267431308732</v>
+        <v>-0.003756267431308731</v>
       </c>
       <c r="I13" t="n">
-        <v>0.05400895170944195</v>
+        <v>0.05400895170944196</v>
       </c>
       <c r="J13" t="n">
         <v>0.06973382062536339</v>
       </c>
       <c r="K13" t="n">
-        <v>0.2987826524325735</v>
+        <v>0.2987826524325734</v>
       </c>
       <c r="L13" t="n">
         <v>-0.2799222481290676</v>
@@ -1059,13 +1059,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.08887914460199314</v>
+        <v>-0.08887914460199312</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04279219720910433</v>
+        <v>0.04579195693789806</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.01893148487609337</v>
+        <v>-0.01893148487609338</v>
       </c>
       <c r="E14" t="n">
         <v>-0.1164410583049517</v>
@@ -1077,16 +1077,16 @@
         <v>-0.137159322736744</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0009322909582774888</v>
+        <v>0.0009322909582774932</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.02642557985560759</v>
+        <v>-0.0264255798556076</v>
       </c>
       <c r="J14" t="n">
-        <v>0.01892521710331612</v>
+        <v>0.01892521710331613</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.1653177463296435</v>
+        <v>-0.1653177463296434</v>
       </c>
       <c r="L14" t="n">
         <v>0.7354368068132261</v>

</xml_diff>